<commit_message>
[QSI] Change font size
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/70歳以上被用者不該当届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/70歳以上被用者不該当届_帳票テンプレート.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32E11F6-8C18-4106-9123-7877DB121B24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="資格喪失届" sheetId="2" r:id="rId1"/>
@@ -834,7 +833,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-411]ggg"/>
     <numFmt numFmtId="165" formatCode="00000000;;"/>
@@ -2598,15 +2597,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2703,9 +2693,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma [0] 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma [0] 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -13326,14 +13325,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:EU245"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:AS24"/>
+      <selection activeCell="H13" sqref="H13:AY16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -13355,50 +13354,50 @@
       <c r="U2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="403" t="s">
+      <c r="Y2" s="400" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="403"/>
-      <c r="AA2" s="403"/>
-      <c r="AB2" s="403"/>
-      <c r="AC2" s="403"/>
-      <c r="AD2" s="403"/>
-      <c r="AE2" s="403"/>
-      <c r="AF2" s="403"/>
-      <c r="AG2" s="403"/>
+      <c r="Z2" s="400"/>
+      <c r="AA2" s="400"/>
+      <c r="AB2" s="400"/>
+      <c r="AC2" s="400"/>
+      <c r="AD2" s="400"/>
+      <c r="AE2" s="400"/>
+      <c r="AF2" s="400"/>
+      <c r="AG2" s="400"/>
       <c r="AH2" s="3"/>
-      <c r="AI2" s="401" t="s">
+      <c r="AI2" s="398" t="s">
         <v>1</v>
       </c>
-      <c r="AJ2" s="401"/>
-      <c r="AK2" s="401"/>
-      <c r="AL2" s="401"/>
-      <c r="AM2" s="401"/>
-      <c r="AN2" s="401"/>
-      <c r="AO2" s="401"/>
-      <c r="AP2" s="401"/>
-      <c r="AQ2" s="401"/>
-      <c r="AR2" s="401"/>
-      <c r="AS2" s="401"/>
-      <c r="AT2" s="401"/>
-      <c r="AU2" s="401"/>
-      <c r="AV2" s="401"/>
-      <c r="AW2" s="401"/>
-      <c r="AX2" s="401"/>
-      <c r="AY2" s="401"/>
-      <c r="AZ2" s="401"/>
-      <c r="BA2" s="401"/>
-      <c r="BB2" s="401"/>
-      <c r="BC2" s="401"/>
-      <c r="BD2" s="401"/>
-      <c r="BE2" s="401"/>
-      <c r="BF2" s="401"/>
-      <c r="BG2" s="401"/>
-      <c r="BH2" s="401"/>
-      <c r="BI2" s="401"/>
-      <c r="BJ2" s="401"/>
-      <c r="BK2" s="401"/>
-      <c r="BL2" s="401"/>
+      <c r="AJ2" s="398"/>
+      <c r="AK2" s="398"/>
+      <c r="AL2" s="398"/>
+      <c r="AM2" s="398"/>
+      <c r="AN2" s="398"/>
+      <c r="AO2" s="398"/>
+      <c r="AP2" s="398"/>
+      <c r="AQ2" s="398"/>
+      <c r="AR2" s="398"/>
+      <c r="AS2" s="398"/>
+      <c r="AT2" s="398"/>
+      <c r="AU2" s="398"/>
+      <c r="AV2" s="398"/>
+      <c r="AW2" s="398"/>
+      <c r="AX2" s="398"/>
+      <c r="AY2" s="398"/>
+      <c r="AZ2" s="398"/>
+      <c r="BA2" s="398"/>
+      <c r="BB2" s="398"/>
+      <c r="BC2" s="398"/>
+      <c r="BD2" s="398"/>
+      <c r="BE2" s="398"/>
+      <c r="BF2" s="398"/>
+      <c r="BG2" s="398"/>
+      <c r="BH2" s="398"/>
+      <c r="BI2" s="398"/>
+      <c r="BJ2" s="398"/>
+      <c r="BK2" s="398"/>
+      <c r="BL2" s="398"/>
       <c r="BN2" s="4"/>
       <c r="BO2" s="4"/>
     </row>
@@ -13407,46 +13406,46 @@
       <c r="U3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
-      <c r="Y3" s="404" t="s">
+      <c r="Y3" s="401" t="s">
         <v>2</v>
       </c>
-      <c r="Z3" s="404"/>
-      <c r="AA3" s="404"/>
-      <c r="AB3" s="404"/>
-      <c r="AC3" s="404"/>
-      <c r="AD3" s="404"/>
-      <c r="AE3" s="404"/>
-      <c r="AF3" s="404"/>
-      <c r="AG3" s="404"/>
+      <c r="Z3" s="401"/>
+      <c r="AA3" s="401"/>
+      <c r="AB3" s="401"/>
+      <c r="AC3" s="401"/>
+      <c r="AD3" s="401"/>
+      <c r="AE3" s="401"/>
+      <c r="AF3" s="401"/>
+      <c r="AG3" s="401"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="6"/>
       <c r="AK3" s="6"/>
       <c r="AL3" s="6"/>
-      <c r="AM3" s="402" t="s">
+      <c r="AM3" s="399" t="s">
         <v>3</v>
       </c>
-      <c r="AN3" s="402"/>
-      <c r="AO3" s="402"/>
-      <c r="AP3" s="402"/>
-      <c r="AQ3" s="402"/>
-      <c r="AR3" s="402"/>
-      <c r="AS3" s="402"/>
-      <c r="AT3" s="402"/>
-      <c r="AU3" s="402"/>
-      <c r="AV3" s="402"/>
-      <c r="AW3" s="402"/>
-      <c r="AX3" s="402"/>
-      <c r="AY3" s="402"/>
-      <c r="AZ3" s="402"/>
-      <c r="BA3" s="402"/>
-      <c r="BB3" s="402"/>
-      <c r="BC3" s="402"/>
-      <c r="BD3" s="402"/>
-      <c r="BE3" s="402"/>
-      <c r="BF3" s="402"/>
-      <c r="BG3" s="402"/>
-      <c r="BH3" s="402"/>
+      <c r="AN3" s="399"/>
+      <c r="AO3" s="399"/>
+      <c r="AP3" s="399"/>
+      <c r="AQ3" s="399"/>
+      <c r="AR3" s="399"/>
+      <c r="AS3" s="399"/>
+      <c r="AT3" s="399"/>
+      <c r="AU3" s="399"/>
+      <c r="AV3" s="399"/>
+      <c r="AW3" s="399"/>
+      <c r="AX3" s="399"/>
+      <c r="AY3" s="399"/>
+      <c r="AZ3" s="399"/>
+      <c r="BA3" s="399"/>
+      <c r="BB3" s="399"/>
+      <c r="BC3" s="399"/>
+      <c r="BD3" s="399"/>
+      <c r="BE3" s="399"/>
+      <c r="BF3" s="399"/>
+      <c r="BG3" s="399"/>
+      <c r="BH3" s="399"/>
       <c r="BM3" s="126"/>
     </row>
     <row r="4" spans="2:105" ht="8.25" customHeight="1">
@@ -13768,33 +13767,33 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="407" t="s">
+      <c r="H11" s="404" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="408"/>
-      <c r="J11" s="408"/>
-      <c r="K11" s="408"/>
-      <c r="L11" s="408"/>
-      <c r="M11" s="408"/>
-      <c r="N11" s="408"/>
-      <c r="O11" s="408"/>
-      <c r="P11" s="408"/>
-      <c r="Q11" s="408"/>
-      <c r="R11" s="408"/>
-      <c r="S11" s="408"/>
-      <c r="T11" s="408"/>
-      <c r="U11" s="408"/>
-      <c r="V11" s="408"/>
-      <c r="W11" s="408"/>
-      <c r="X11" s="408"/>
-      <c r="Y11" s="408"/>
-      <c r="Z11" s="408"/>
-      <c r="AA11" s="408"/>
-      <c r="AB11" s="408"/>
-      <c r="AC11" s="408"/>
-      <c r="AD11" s="408"/>
-      <c r="AE11" s="408"/>
-      <c r="AF11" s="408"/>
+      <c r="I11" s="405"/>
+      <c r="J11" s="405"/>
+      <c r="K11" s="405"/>
+      <c r="L11" s="405"/>
+      <c r="M11" s="405"/>
+      <c r="N11" s="405"/>
+      <c r="O11" s="405"/>
+      <c r="P11" s="405"/>
+      <c r="Q11" s="405"/>
+      <c r="R11" s="405"/>
+      <c r="S11" s="405"/>
+      <c r="T11" s="405"/>
+      <c r="U11" s="405"/>
+      <c r="V11" s="405"/>
+      <c r="W11" s="405"/>
+      <c r="X11" s="405"/>
+      <c r="Y11" s="405"/>
+      <c r="Z11" s="405"/>
+      <c r="AA11" s="405"/>
+      <c r="AB11" s="405"/>
+      <c r="AC11" s="405"/>
+      <c r="AD11" s="405"/>
+      <c r="AE11" s="405"/>
+      <c r="AF11" s="405"/>
       <c r="AG11" s="16"/>
       <c r="AH11" s="16"/>
       <c r="AI11" s="16"/>
@@ -13850,28 +13849,28 @@
       <c r="E12" s="386"/>
       <c r="F12" s="386"/>
       <c r="G12" s="387"/>
-      <c r="H12" s="416" t="s">
+      <c r="H12" s="413" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="417"/>
-      <c r="J12" s="400"/>
-      <c r="K12" s="400"/>
-      <c r="L12" s="400"/>
-      <c r="M12" s="400"/>
-      <c r="N12" s="400"/>
-      <c r="O12" s="400"/>
-      <c r="P12" s="417" t="s">
+      <c r="I12" s="414"/>
+      <c r="J12" s="397"/>
+      <c r="K12" s="397"/>
+      <c r="L12" s="397"/>
+      <c r="M12" s="397"/>
+      <c r="N12" s="397"/>
+      <c r="O12" s="397"/>
+      <c r="P12" s="414" t="s">
         <v>25</v>
       </c>
-      <c r="Q12" s="417"/>
-      <c r="R12" s="400"/>
-      <c r="S12" s="400"/>
-      <c r="T12" s="400"/>
-      <c r="U12" s="400"/>
-      <c r="V12" s="400"/>
-      <c r="W12" s="400"/>
-      <c r="X12" s="400"/>
-      <c r="Y12" s="400"/>
+      <c r="Q12" s="414"/>
+      <c r="R12" s="397"/>
+      <c r="S12" s="397"/>
+      <c r="T12" s="397"/>
+      <c r="U12" s="397"/>
+      <c r="V12" s="397"/>
+      <c r="W12" s="397"/>
+      <c r="X12" s="397"/>
+      <c r="Y12" s="397"/>
       <c r="Z12" s="19"/>
       <c r="AA12" s="19"/>
       <c r="AB12" s="19"/>
@@ -13932,50 +13931,50 @@
       <c r="E13" s="386"/>
       <c r="F13" s="386"/>
       <c r="G13" s="387"/>
-      <c r="H13" s="388"/>
-      <c r="I13" s="389"/>
-      <c r="J13" s="389"/>
-      <c r="K13" s="389"/>
-      <c r="L13" s="389"/>
-      <c r="M13" s="389"/>
-      <c r="N13" s="389"/>
-      <c r="O13" s="389"/>
-      <c r="P13" s="389"/>
-      <c r="Q13" s="389"/>
-      <c r="R13" s="389"/>
-      <c r="S13" s="389"/>
-      <c r="T13" s="389"/>
-      <c r="U13" s="389"/>
-      <c r="V13" s="389"/>
-      <c r="W13" s="389"/>
-      <c r="X13" s="389"/>
-      <c r="Y13" s="389"/>
-      <c r="Z13" s="389"/>
-      <c r="AA13" s="389"/>
-      <c r="AB13" s="389"/>
-      <c r="AC13" s="389"/>
-      <c r="AD13" s="389"/>
-      <c r="AE13" s="389"/>
-      <c r="AF13" s="389"/>
-      <c r="AG13" s="389"/>
-      <c r="AH13" s="389"/>
-      <c r="AI13" s="389"/>
-      <c r="AJ13" s="389"/>
-      <c r="AK13" s="389"/>
-      <c r="AL13" s="389"/>
-      <c r="AM13" s="389"/>
-      <c r="AN13" s="389"/>
-      <c r="AO13" s="389"/>
-      <c r="AP13" s="389"/>
-      <c r="AQ13" s="389"/>
-      <c r="AR13" s="389"/>
-      <c r="AS13" s="389"/>
-      <c r="AT13" s="389"/>
-      <c r="AU13" s="389"/>
-      <c r="AV13" s="389"/>
-      <c r="AW13" s="389"/>
-      <c r="AX13" s="389"/>
-      <c r="AY13" s="390"/>
+      <c r="H13" s="420"/>
+      <c r="I13" s="421"/>
+      <c r="J13" s="421"/>
+      <c r="K13" s="421"/>
+      <c r="L13" s="421"/>
+      <c r="M13" s="421"/>
+      <c r="N13" s="421"/>
+      <c r="O13" s="421"/>
+      <c r="P13" s="421"/>
+      <c r="Q13" s="421"/>
+      <c r="R13" s="421"/>
+      <c r="S13" s="421"/>
+      <c r="T13" s="421"/>
+      <c r="U13" s="421"/>
+      <c r="V13" s="421"/>
+      <c r="W13" s="421"/>
+      <c r="X13" s="421"/>
+      <c r="Y13" s="421"/>
+      <c r="Z13" s="421"/>
+      <c r="AA13" s="421"/>
+      <c r="AB13" s="421"/>
+      <c r="AC13" s="421"/>
+      <c r="AD13" s="421"/>
+      <c r="AE13" s="421"/>
+      <c r="AF13" s="421"/>
+      <c r="AG13" s="421"/>
+      <c r="AH13" s="421"/>
+      <c r="AI13" s="421"/>
+      <c r="AJ13" s="421"/>
+      <c r="AK13" s="421"/>
+      <c r="AL13" s="421"/>
+      <c r="AM13" s="421"/>
+      <c r="AN13" s="421"/>
+      <c r="AO13" s="421"/>
+      <c r="AP13" s="421"/>
+      <c r="AQ13" s="421"/>
+      <c r="AR13" s="421"/>
+      <c r="AS13" s="421"/>
+      <c r="AT13" s="421"/>
+      <c r="AU13" s="421"/>
+      <c r="AV13" s="421"/>
+      <c r="AW13" s="421"/>
+      <c r="AX13" s="421"/>
+      <c r="AY13" s="422"/>
       <c r="AZ13" s="20"/>
       <c r="BA13" s="10"/>
       <c r="BB13" s="10"/>
@@ -14010,50 +14009,50 @@
       <c r="E14" s="386"/>
       <c r="F14" s="386"/>
       <c r="G14" s="387"/>
-      <c r="H14" s="388"/>
-      <c r="I14" s="389"/>
-      <c r="J14" s="389"/>
-      <c r="K14" s="389"/>
-      <c r="L14" s="389"/>
-      <c r="M14" s="389"/>
-      <c r="N14" s="389"/>
-      <c r="O14" s="389"/>
-      <c r="P14" s="389"/>
-      <c r="Q14" s="389"/>
-      <c r="R14" s="389"/>
-      <c r="S14" s="389"/>
-      <c r="T14" s="389"/>
-      <c r="U14" s="389"/>
-      <c r="V14" s="389"/>
-      <c r="W14" s="389"/>
-      <c r="X14" s="389"/>
-      <c r="Y14" s="389"/>
-      <c r="Z14" s="389"/>
-      <c r="AA14" s="389"/>
-      <c r="AB14" s="389"/>
-      <c r="AC14" s="389"/>
-      <c r="AD14" s="389"/>
-      <c r="AE14" s="389"/>
-      <c r="AF14" s="389"/>
-      <c r="AG14" s="389"/>
-      <c r="AH14" s="389"/>
-      <c r="AI14" s="389"/>
-      <c r="AJ14" s="389"/>
-      <c r="AK14" s="389"/>
-      <c r="AL14" s="389"/>
-      <c r="AM14" s="389"/>
-      <c r="AN14" s="389"/>
-      <c r="AO14" s="389"/>
-      <c r="AP14" s="389"/>
-      <c r="AQ14" s="389"/>
-      <c r="AR14" s="389"/>
-      <c r="AS14" s="389"/>
-      <c r="AT14" s="389"/>
-      <c r="AU14" s="389"/>
-      <c r="AV14" s="389"/>
-      <c r="AW14" s="389"/>
-      <c r="AX14" s="389"/>
-      <c r="AY14" s="390"/>
+      <c r="H14" s="420"/>
+      <c r="I14" s="421"/>
+      <c r="J14" s="421"/>
+      <c r="K14" s="421"/>
+      <c r="L14" s="421"/>
+      <c r="M14" s="421"/>
+      <c r="N14" s="421"/>
+      <c r="O14" s="421"/>
+      <c r="P14" s="421"/>
+      <c r="Q14" s="421"/>
+      <c r="R14" s="421"/>
+      <c r="S14" s="421"/>
+      <c r="T14" s="421"/>
+      <c r="U14" s="421"/>
+      <c r="V14" s="421"/>
+      <c r="W14" s="421"/>
+      <c r="X14" s="421"/>
+      <c r="Y14" s="421"/>
+      <c r="Z14" s="421"/>
+      <c r="AA14" s="421"/>
+      <c r="AB14" s="421"/>
+      <c r="AC14" s="421"/>
+      <c r="AD14" s="421"/>
+      <c r="AE14" s="421"/>
+      <c r="AF14" s="421"/>
+      <c r="AG14" s="421"/>
+      <c r="AH14" s="421"/>
+      <c r="AI14" s="421"/>
+      <c r="AJ14" s="421"/>
+      <c r="AK14" s="421"/>
+      <c r="AL14" s="421"/>
+      <c r="AM14" s="421"/>
+      <c r="AN14" s="421"/>
+      <c r="AO14" s="421"/>
+      <c r="AP14" s="421"/>
+      <c r="AQ14" s="421"/>
+      <c r="AR14" s="421"/>
+      <c r="AS14" s="421"/>
+      <c r="AT14" s="421"/>
+      <c r="AU14" s="421"/>
+      <c r="AV14" s="421"/>
+      <c r="AW14" s="421"/>
+      <c r="AX14" s="421"/>
+      <c r="AY14" s="422"/>
       <c r="AZ14" s="20"/>
       <c r="BA14" s="10"/>
       <c r="BB14" s="10"/>
@@ -14084,50 +14083,50 @@
       <c r="E15" s="386"/>
       <c r="F15" s="386"/>
       <c r="G15" s="387"/>
-      <c r="H15" s="388"/>
-      <c r="I15" s="389"/>
-      <c r="J15" s="389"/>
-      <c r="K15" s="389"/>
-      <c r="L15" s="389"/>
-      <c r="M15" s="389"/>
-      <c r="N15" s="389"/>
-      <c r="O15" s="389"/>
-      <c r="P15" s="389"/>
-      <c r="Q15" s="389"/>
-      <c r="R15" s="389"/>
-      <c r="S15" s="389"/>
-      <c r="T15" s="389"/>
-      <c r="U15" s="389"/>
-      <c r="V15" s="389"/>
-      <c r="W15" s="389"/>
-      <c r="X15" s="389"/>
-      <c r="Y15" s="389"/>
-      <c r="Z15" s="389"/>
-      <c r="AA15" s="389"/>
-      <c r="AB15" s="389"/>
-      <c r="AC15" s="389"/>
-      <c r="AD15" s="389"/>
-      <c r="AE15" s="389"/>
-      <c r="AF15" s="389"/>
-      <c r="AG15" s="389"/>
-      <c r="AH15" s="389"/>
-      <c r="AI15" s="389"/>
-      <c r="AJ15" s="389"/>
-      <c r="AK15" s="389"/>
-      <c r="AL15" s="389"/>
-      <c r="AM15" s="389"/>
-      <c r="AN15" s="389"/>
-      <c r="AO15" s="389"/>
-      <c r="AP15" s="389"/>
-      <c r="AQ15" s="389"/>
-      <c r="AR15" s="389"/>
-      <c r="AS15" s="389"/>
-      <c r="AT15" s="389"/>
-      <c r="AU15" s="389"/>
-      <c r="AV15" s="389"/>
-      <c r="AW15" s="389"/>
-      <c r="AX15" s="389"/>
-      <c r="AY15" s="390"/>
+      <c r="H15" s="420"/>
+      <c r="I15" s="421"/>
+      <c r="J15" s="421"/>
+      <c r="K15" s="421"/>
+      <c r="L15" s="421"/>
+      <c r="M15" s="421"/>
+      <c r="N15" s="421"/>
+      <c r="O15" s="421"/>
+      <c r="P15" s="421"/>
+      <c r="Q15" s="421"/>
+      <c r="R15" s="421"/>
+      <c r="S15" s="421"/>
+      <c r="T15" s="421"/>
+      <c r="U15" s="421"/>
+      <c r="V15" s="421"/>
+      <c r="W15" s="421"/>
+      <c r="X15" s="421"/>
+      <c r="Y15" s="421"/>
+      <c r="Z15" s="421"/>
+      <c r="AA15" s="421"/>
+      <c r="AB15" s="421"/>
+      <c r="AC15" s="421"/>
+      <c r="AD15" s="421"/>
+      <c r="AE15" s="421"/>
+      <c r="AF15" s="421"/>
+      <c r="AG15" s="421"/>
+      <c r="AH15" s="421"/>
+      <c r="AI15" s="421"/>
+      <c r="AJ15" s="421"/>
+      <c r="AK15" s="421"/>
+      <c r="AL15" s="421"/>
+      <c r="AM15" s="421"/>
+      <c r="AN15" s="421"/>
+      <c r="AO15" s="421"/>
+      <c r="AP15" s="421"/>
+      <c r="AQ15" s="421"/>
+      <c r="AR15" s="421"/>
+      <c r="AS15" s="421"/>
+      <c r="AT15" s="421"/>
+      <c r="AU15" s="421"/>
+      <c r="AV15" s="421"/>
+      <c r="AW15" s="421"/>
+      <c r="AX15" s="421"/>
+      <c r="AY15" s="422"/>
       <c r="AZ15" s="20"/>
       <c r="BA15" s="10"/>
       <c r="BB15" s="10"/>
@@ -14158,50 +14157,50 @@
       <c r="E16" s="386"/>
       <c r="F16" s="386"/>
       <c r="G16" s="387"/>
-      <c r="H16" s="388"/>
-      <c r="I16" s="389"/>
-      <c r="J16" s="389"/>
-      <c r="K16" s="389"/>
-      <c r="L16" s="389"/>
-      <c r="M16" s="389"/>
-      <c r="N16" s="389"/>
-      <c r="O16" s="389"/>
-      <c r="P16" s="389"/>
-      <c r="Q16" s="389"/>
-      <c r="R16" s="389"/>
-      <c r="S16" s="389"/>
-      <c r="T16" s="389"/>
-      <c r="U16" s="389"/>
-      <c r="V16" s="389"/>
-      <c r="W16" s="389"/>
-      <c r="X16" s="389"/>
-      <c r="Y16" s="389"/>
-      <c r="Z16" s="389"/>
-      <c r="AA16" s="389"/>
-      <c r="AB16" s="389"/>
-      <c r="AC16" s="389"/>
-      <c r="AD16" s="389"/>
-      <c r="AE16" s="389"/>
-      <c r="AF16" s="389"/>
-      <c r="AG16" s="389"/>
-      <c r="AH16" s="389"/>
-      <c r="AI16" s="389"/>
-      <c r="AJ16" s="389"/>
-      <c r="AK16" s="389"/>
-      <c r="AL16" s="389"/>
-      <c r="AM16" s="389"/>
-      <c r="AN16" s="389"/>
-      <c r="AO16" s="389"/>
-      <c r="AP16" s="389"/>
-      <c r="AQ16" s="389"/>
-      <c r="AR16" s="389"/>
-      <c r="AS16" s="389"/>
-      <c r="AT16" s="389"/>
-      <c r="AU16" s="389"/>
-      <c r="AV16" s="389"/>
-      <c r="AW16" s="389"/>
-      <c r="AX16" s="389"/>
-      <c r="AY16" s="390"/>
+      <c r="H16" s="420"/>
+      <c r="I16" s="421"/>
+      <c r="J16" s="421"/>
+      <c r="K16" s="421"/>
+      <c r="L16" s="421"/>
+      <c r="M16" s="421"/>
+      <c r="N16" s="421"/>
+      <c r="O16" s="421"/>
+      <c r="P16" s="421"/>
+      <c r="Q16" s="421"/>
+      <c r="R16" s="421"/>
+      <c r="S16" s="421"/>
+      <c r="T16" s="421"/>
+      <c r="U16" s="421"/>
+      <c r="V16" s="421"/>
+      <c r="W16" s="421"/>
+      <c r="X16" s="421"/>
+      <c r="Y16" s="421"/>
+      <c r="Z16" s="421"/>
+      <c r="AA16" s="421"/>
+      <c r="AB16" s="421"/>
+      <c r="AC16" s="421"/>
+      <c r="AD16" s="421"/>
+      <c r="AE16" s="421"/>
+      <c r="AF16" s="421"/>
+      <c r="AG16" s="421"/>
+      <c r="AH16" s="421"/>
+      <c r="AI16" s="421"/>
+      <c r="AJ16" s="421"/>
+      <c r="AK16" s="421"/>
+      <c r="AL16" s="421"/>
+      <c r="AM16" s="421"/>
+      <c r="AN16" s="421"/>
+      <c r="AO16" s="421"/>
+      <c r="AP16" s="421"/>
+      <c r="AQ16" s="421"/>
+      <c r="AR16" s="421"/>
+      <c r="AS16" s="421"/>
+      <c r="AT16" s="421"/>
+      <c r="AU16" s="421"/>
+      <c r="AV16" s="421"/>
+      <c r="AW16" s="421"/>
+      <c r="AX16" s="421"/>
+      <c r="AY16" s="422"/>
       <c r="AZ16" s="20"/>
       <c r="BA16" s="10"/>
       <c r="BB16" s="10"/>
@@ -14234,50 +14233,50 @@
       <c r="E17" s="386"/>
       <c r="F17" s="386"/>
       <c r="G17" s="387"/>
-      <c r="H17" s="391"/>
-      <c r="I17" s="392"/>
-      <c r="J17" s="392"/>
-      <c r="K17" s="392"/>
-      <c r="L17" s="392"/>
-      <c r="M17" s="392"/>
-      <c r="N17" s="392"/>
-      <c r="O17" s="392"/>
-      <c r="P17" s="392"/>
-      <c r="Q17" s="392"/>
-      <c r="R17" s="392"/>
-      <c r="S17" s="392"/>
-      <c r="T17" s="392"/>
-      <c r="U17" s="392"/>
-      <c r="V17" s="392"/>
-      <c r="W17" s="392"/>
-      <c r="X17" s="392"/>
-      <c r="Y17" s="392"/>
-      <c r="Z17" s="392"/>
-      <c r="AA17" s="392"/>
-      <c r="AB17" s="392"/>
-      <c r="AC17" s="392"/>
-      <c r="AD17" s="392"/>
-      <c r="AE17" s="392"/>
-      <c r="AF17" s="392"/>
-      <c r="AG17" s="392"/>
-      <c r="AH17" s="392"/>
-      <c r="AI17" s="392"/>
-      <c r="AJ17" s="392"/>
-      <c r="AK17" s="392"/>
-      <c r="AL17" s="392"/>
-      <c r="AM17" s="392"/>
-      <c r="AN17" s="392"/>
-      <c r="AO17" s="392"/>
-      <c r="AP17" s="392"/>
-      <c r="AQ17" s="392"/>
-      <c r="AR17" s="392"/>
-      <c r="AS17" s="392"/>
-      <c r="AT17" s="392"/>
-      <c r="AU17" s="392"/>
-      <c r="AV17" s="392"/>
-      <c r="AW17" s="392"/>
-      <c r="AX17" s="392"/>
-      <c r="AY17" s="393"/>
+      <c r="H17" s="388"/>
+      <c r="I17" s="389"/>
+      <c r="J17" s="389"/>
+      <c r="K17" s="389"/>
+      <c r="L17" s="389"/>
+      <c r="M17" s="389"/>
+      <c r="N17" s="389"/>
+      <c r="O17" s="389"/>
+      <c r="P17" s="389"/>
+      <c r="Q17" s="389"/>
+      <c r="R17" s="389"/>
+      <c r="S17" s="389"/>
+      <c r="T17" s="389"/>
+      <c r="U17" s="389"/>
+      <c r="V17" s="389"/>
+      <c r="W17" s="389"/>
+      <c r="X17" s="389"/>
+      <c r="Y17" s="389"/>
+      <c r="Z17" s="389"/>
+      <c r="AA17" s="389"/>
+      <c r="AB17" s="389"/>
+      <c r="AC17" s="389"/>
+      <c r="AD17" s="389"/>
+      <c r="AE17" s="389"/>
+      <c r="AF17" s="389"/>
+      <c r="AG17" s="389"/>
+      <c r="AH17" s="389"/>
+      <c r="AI17" s="389"/>
+      <c r="AJ17" s="389"/>
+      <c r="AK17" s="389"/>
+      <c r="AL17" s="389"/>
+      <c r="AM17" s="389"/>
+      <c r="AN17" s="389"/>
+      <c r="AO17" s="389"/>
+      <c r="AP17" s="389"/>
+      <c r="AQ17" s="389"/>
+      <c r="AR17" s="389"/>
+      <c r="AS17" s="389"/>
+      <c r="AT17" s="389"/>
+      <c r="AU17" s="389"/>
+      <c r="AV17" s="389"/>
+      <c r="AW17" s="389"/>
+      <c r="AX17" s="389"/>
+      <c r="AY17" s="390"/>
       <c r="AZ17" s="20"/>
       <c r="BA17" s="10"/>
       <c r="BB17" s="10"/>
@@ -14308,50 +14307,50 @@
       <c r="E18" s="386"/>
       <c r="F18" s="386"/>
       <c r="G18" s="387"/>
-      <c r="H18" s="391"/>
-      <c r="I18" s="392"/>
-      <c r="J18" s="392"/>
-      <c r="K18" s="392"/>
-      <c r="L18" s="392"/>
-      <c r="M18" s="392"/>
-      <c r="N18" s="392"/>
-      <c r="O18" s="392"/>
-      <c r="P18" s="392"/>
-      <c r="Q18" s="392"/>
-      <c r="R18" s="392"/>
-      <c r="S18" s="392"/>
-      <c r="T18" s="392"/>
-      <c r="U18" s="392"/>
-      <c r="V18" s="392"/>
-      <c r="W18" s="392"/>
-      <c r="X18" s="392"/>
-      <c r="Y18" s="392"/>
-      <c r="Z18" s="392"/>
-      <c r="AA18" s="392"/>
-      <c r="AB18" s="392"/>
-      <c r="AC18" s="392"/>
-      <c r="AD18" s="392"/>
-      <c r="AE18" s="392"/>
-      <c r="AF18" s="392"/>
-      <c r="AG18" s="392"/>
-      <c r="AH18" s="392"/>
-      <c r="AI18" s="392"/>
-      <c r="AJ18" s="392"/>
-      <c r="AK18" s="392"/>
-      <c r="AL18" s="392"/>
-      <c r="AM18" s="392"/>
-      <c r="AN18" s="392"/>
-      <c r="AO18" s="392"/>
-      <c r="AP18" s="392"/>
-      <c r="AQ18" s="392"/>
-      <c r="AR18" s="392"/>
-      <c r="AS18" s="392"/>
-      <c r="AT18" s="392"/>
-      <c r="AU18" s="392"/>
-      <c r="AV18" s="392"/>
-      <c r="AW18" s="392"/>
-      <c r="AX18" s="392"/>
-      <c r="AY18" s="393"/>
+      <c r="H18" s="388"/>
+      <c r="I18" s="389"/>
+      <c r="J18" s="389"/>
+      <c r="K18" s="389"/>
+      <c r="L18" s="389"/>
+      <c r="M18" s="389"/>
+      <c r="N18" s="389"/>
+      <c r="O18" s="389"/>
+      <c r="P18" s="389"/>
+      <c r="Q18" s="389"/>
+      <c r="R18" s="389"/>
+      <c r="S18" s="389"/>
+      <c r="T18" s="389"/>
+      <c r="U18" s="389"/>
+      <c r="V18" s="389"/>
+      <c r="W18" s="389"/>
+      <c r="X18" s="389"/>
+      <c r="Y18" s="389"/>
+      <c r="Z18" s="389"/>
+      <c r="AA18" s="389"/>
+      <c r="AB18" s="389"/>
+      <c r="AC18" s="389"/>
+      <c r="AD18" s="389"/>
+      <c r="AE18" s="389"/>
+      <c r="AF18" s="389"/>
+      <c r="AG18" s="389"/>
+      <c r="AH18" s="389"/>
+      <c r="AI18" s="389"/>
+      <c r="AJ18" s="389"/>
+      <c r="AK18" s="389"/>
+      <c r="AL18" s="389"/>
+      <c r="AM18" s="389"/>
+      <c r="AN18" s="389"/>
+      <c r="AO18" s="389"/>
+      <c r="AP18" s="389"/>
+      <c r="AQ18" s="389"/>
+      <c r="AR18" s="389"/>
+      <c r="AS18" s="389"/>
+      <c r="AT18" s="389"/>
+      <c r="AU18" s="389"/>
+      <c r="AV18" s="389"/>
+      <c r="AW18" s="389"/>
+      <c r="AX18" s="389"/>
+      <c r="AY18" s="390"/>
       <c r="AZ18" s="20"/>
       <c r="BA18" s="10"/>
       <c r="BB18" s="10"/>
@@ -14382,50 +14381,50 @@
       <c r="E19" s="386"/>
       <c r="F19" s="386"/>
       <c r="G19" s="387"/>
-      <c r="H19" s="391"/>
-      <c r="I19" s="392"/>
-      <c r="J19" s="392"/>
-      <c r="K19" s="392"/>
-      <c r="L19" s="392"/>
-      <c r="M19" s="392"/>
-      <c r="N19" s="392"/>
-      <c r="O19" s="392"/>
-      <c r="P19" s="392"/>
-      <c r="Q19" s="392"/>
-      <c r="R19" s="392"/>
-      <c r="S19" s="392"/>
-      <c r="T19" s="392"/>
-      <c r="U19" s="392"/>
-      <c r="V19" s="392"/>
-      <c r="W19" s="392"/>
-      <c r="X19" s="392"/>
-      <c r="Y19" s="392"/>
-      <c r="Z19" s="392"/>
-      <c r="AA19" s="392"/>
-      <c r="AB19" s="392"/>
-      <c r="AC19" s="392"/>
-      <c r="AD19" s="392"/>
-      <c r="AE19" s="392"/>
-      <c r="AF19" s="392"/>
-      <c r="AG19" s="392"/>
-      <c r="AH19" s="392"/>
-      <c r="AI19" s="392"/>
-      <c r="AJ19" s="392"/>
-      <c r="AK19" s="392"/>
-      <c r="AL19" s="392"/>
-      <c r="AM19" s="392"/>
-      <c r="AN19" s="392"/>
-      <c r="AO19" s="392"/>
-      <c r="AP19" s="392"/>
-      <c r="AQ19" s="392"/>
-      <c r="AR19" s="392"/>
-      <c r="AS19" s="392"/>
-      <c r="AT19" s="392"/>
-      <c r="AU19" s="392"/>
-      <c r="AV19" s="392"/>
-      <c r="AW19" s="392"/>
-      <c r="AX19" s="392"/>
-      <c r="AY19" s="393"/>
+      <c r="H19" s="388"/>
+      <c r="I19" s="389"/>
+      <c r="J19" s="389"/>
+      <c r="K19" s="389"/>
+      <c r="L19" s="389"/>
+      <c r="M19" s="389"/>
+      <c r="N19" s="389"/>
+      <c r="O19" s="389"/>
+      <c r="P19" s="389"/>
+      <c r="Q19" s="389"/>
+      <c r="R19" s="389"/>
+      <c r="S19" s="389"/>
+      <c r="T19" s="389"/>
+      <c r="U19" s="389"/>
+      <c r="V19" s="389"/>
+      <c r="W19" s="389"/>
+      <c r="X19" s="389"/>
+      <c r="Y19" s="389"/>
+      <c r="Z19" s="389"/>
+      <c r="AA19" s="389"/>
+      <c r="AB19" s="389"/>
+      <c r="AC19" s="389"/>
+      <c r="AD19" s="389"/>
+      <c r="AE19" s="389"/>
+      <c r="AF19" s="389"/>
+      <c r="AG19" s="389"/>
+      <c r="AH19" s="389"/>
+      <c r="AI19" s="389"/>
+      <c r="AJ19" s="389"/>
+      <c r="AK19" s="389"/>
+      <c r="AL19" s="389"/>
+      <c r="AM19" s="389"/>
+      <c r="AN19" s="389"/>
+      <c r="AO19" s="389"/>
+      <c r="AP19" s="389"/>
+      <c r="AQ19" s="389"/>
+      <c r="AR19" s="389"/>
+      <c r="AS19" s="389"/>
+      <c r="AT19" s="389"/>
+      <c r="AU19" s="389"/>
+      <c r="AV19" s="389"/>
+      <c r="AW19" s="389"/>
+      <c r="AX19" s="389"/>
+      <c r="AY19" s="390"/>
       <c r="AZ19" s="20"/>
       <c r="BA19" s="20"/>
       <c r="BD19" s="23"/>
@@ -14462,72 +14461,72 @@
       <c r="E20" s="386"/>
       <c r="F20" s="386"/>
       <c r="G20" s="387"/>
-      <c r="H20" s="391"/>
-      <c r="I20" s="392"/>
-      <c r="J20" s="392"/>
-      <c r="K20" s="392"/>
-      <c r="L20" s="392"/>
-      <c r="M20" s="392"/>
-      <c r="N20" s="392"/>
-      <c r="O20" s="392"/>
-      <c r="P20" s="392"/>
-      <c r="Q20" s="392"/>
-      <c r="R20" s="392"/>
-      <c r="S20" s="392"/>
-      <c r="T20" s="392"/>
-      <c r="U20" s="392"/>
-      <c r="V20" s="392"/>
-      <c r="W20" s="392"/>
-      <c r="X20" s="392"/>
-      <c r="Y20" s="392"/>
-      <c r="Z20" s="392"/>
-      <c r="AA20" s="392"/>
-      <c r="AB20" s="392"/>
-      <c r="AC20" s="392"/>
-      <c r="AD20" s="392"/>
-      <c r="AE20" s="392"/>
-      <c r="AF20" s="392"/>
-      <c r="AG20" s="392"/>
-      <c r="AH20" s="392"/>
-      <c r="AI20" s="392"/>
-      <c r="AJ20" s="392"/>
-      <c r="AK20" s="392"/>
-      <c r="AL20" s="392"/>
-      <c r="AM20" s="392"/>
-      <c r="AN20" s="392"/>
-      <c r="AO20" s="392"/>
-      <c r="AP20" s="392"/>
-      <c r="AQ20" s="392"/>
-      <c r="AR20" s="392"/>
-      <c r="AS20" s="392"/>
-      <c r="AT20" s="392"/>
-      <c r="AU20" s="392"/>
-      <c r="AV20" s="392"/>
-      <c r="AW20" s="392"/>
-      <c r="AX20" s="392"/>
-      <c r="AY20" s="393"/>
+      <c r="H20" s="388"/>
+      <c r="I20" s="389"/>
+      <c r="J20" s="389"/>
+      <c r="K20" s="389"/>
+      <c r="L20" s="389"/>
+      <c r="M20" s="389"/>
+      <c r="N20" s="389"/>
+      <c r="O20" s="389"/>
+      <c r="P20" s="389"/>
+      <c r="Q20" s="389"/>
+      <c r="R20" s="389"/>
+      <c r="S20" s="389"/>
+      <c r="T20" s="389"/>
+      <c r="U20" s="389"/>
+      <c r="V20" s="389"/>
+      <c r="W20" s="389"/>
+      <c r="X20" s="389"/>
+      <c r="Y20" s="389"/>
+      <c r="Z20" s="389"/>
+      <c r="AA20" s="389"/>
+      <c r="AB20" s="389"/>
+      <c r="AC20" s="389"/>
+      <c r="AD20" s="389"/>
+      <c r="AE20" s="389"/>
+      <c r="AF20" s="389"/>
+      <c r="AG20" s="389"/>
+      <c r="AH20" s="389"/>
+      <c r="AI20" s="389"/>
+      <c r="AJ20" s="389"/>
+      <c r="AK20" s="389"/>
+      <c r="AL20" s="389"/>
+      <c r="AM20" s="389"/>
+      <c r="AN20" s="389"/>
+      <c r="AO20" s="389"/>
+      <c r="AP20" s="389"/>
+      <c r="AQ20" s="389"/>
+      <c r="AR20" s="389"/>
+      <c r="AS20" s="389"/>
+      <c r="AT20" s="389"/>
+      <c r="AU20" s="389"/>
+      <c r="AV20" s="389"/>
+      <c r="AW20" s="389"/>
+      <c r="AX20" s="389"/>
+      <c r="AY20" s="390"/>
       <c r="AZ20" s="20"/>
       <c r="BA20" s="20"/>
-      <c r="BD20" s="409" t="s">
+      <c r="BD20" s="406" t="s">
         <v>91</v>
       </c>
-      <c r="BE20" s="410"/>
-      <c r="BF20" s="410"/>
-      <c r="BG20" s="410"/>
-      <c r="BH20" s="410"/>
-      <c r="BI20" s="410"/>
-      <c r="BJ20" s="410"/>
-      <c r="BK20" s="410"/>
-      <c r="BL20" s="410"/>
-      <c r="BM20" s="410"/>
-      <c r="BN20" s="410"/>
-      <c r="BO20" s="410"/>
-      <c r="BP20" s="410"/>
-      <c r="BQ20" s="410"/>
-      <c r="BR20" s="410"/>
-      <c r="BS20" s="410"/>
-      <c r="BT20" s="410"/>
-      <c r="BU20" s="411"/>
+      <c r="BE20" s="407"/>
+      <c r="BF20" s="407"/>
+      <c r="BG20" s="407"/>
+      <c r="BH20" s="407"/>
+      <c r="BI20" s="407"/>
+      <c r="BJ20" s="407"/>
+      <c r="BK20" s="407"/>
+      <c r="BL20" s="407"/>
+      <c r="BM20" s="407"/>
+      <c r="BN20" s="407"/>
+      <c r="BO20" s="407"/>
+      <c r="BP20" s="407"/>
+      <c r="BQ20" s="407"/>
+      <c r="BR20" s="407"/>
+      <c r="BS20" s="407"/>
+      <c r="BT20" s="407"/>
+      <c r="BU20" s="408"/>
       <c r="BV20" s="24"/>
       <c r="BW20" s="24"/>
       <c r="BX20" s="24"/>
@@ -14546,72 +14545,72 @@
       <c r="E21" s="386"/>
       <c r="F21" s="386"/>
       <c r="G21" s="387"/>
-      <c r="H21" s="391"/>
-      <c r="I21" s="392"/>
-      <c r="J21" s="392"/>
-      <c r="K21" s="392"/>
-      <c r="L21" s="392"/>
-      <c r="M21" s="392"/>
-      <c r="N21" s="392"/>
-      <c r="O21" s="392"/>
-      <c r="P21" s="392"/>
-      <c r="Q21" s="392"/>
-      <c r="R21" s="392"/>
-      <c r="S21" s="392"/>
-      <c r="T21" s="392"/>
-      <c r="U21" s="392"/>
-      <c r="V21" s="392"/>
-      <c r="W21" s="392"/>
-      <c r="X21" s="392"/>
-      <c r="Y21" s="392"/>
-      <c r="Z21" s="392"/>
-      <c r="AA21" s="392"/>
-      <c r="AB21" s="392"/>
-      <c r="AC21" s="392"/>
-      <c r="AD21" s="392"/>
-      <c r="AE21" s="392"/>
-      <c r="AF21" s="392"/>
-      <c r="AG21" s="392"/>
-      <c r="AH21" s="392"/>
-      <c r="AI21" s="392"/>
-      <c r="AJ21" s="392"/>
-      <c r="AK21" s="392"/>
-      <c r="AL21" s="392"/>
-      <c r="AM21" s="392"/>
-      <c r="AN21" s="392"/>
-      <c r="AO21" s="392"/>
-      <c r="AP21" s="392"/>
-      <c r="AQ21" s="392"/>
-      <c r="AR21" s="392"/>
-      <c r="AS21" s="392"/>
-      <c r="AT21" s="396" t="s">
+      <c r="H21" s="388"/>
+      <c r="I21" s="389"/>
+      <c r="J21" s="389"/>
+      <c r="K21" s="389"/>
+      <c r="L21" s="389"/>
+      <c r="M21" s="389"/>
+      <c r="N21" s="389"/>
+      <c r="O21" s="389"/>
+      <c r="P21" s="389"/>
+      <c r="Q21" s="389"/>
+      <c r="R21" s="389"/>
+      <c r="S21" s="389"/>
+      <c r="T21" s="389"/>
+      <c r="U21" s="389"/>
+      <c r="V21" s="389"/>
+      <c r="W21" s="389"/>
+      <c r="X21" s="389"/>
+      <c r="Y21" s="389"/>
+      <c r="Z21" s="389"/>
+      <c r="AA21" s="389"/>
+      <c r="AB21" s="389"/>
+      <c r="AC21" s="389"/>
+      <c r="AD21" s="389"/>
+      <c r="AE21" s="389"/>
+      <c r="AF21" s="389"/>
+      <c r="AG21" s="389"/>
+      <c r="AH21" s="389"/>
+      <c r="AI21" s="389"/>
+      <c r="AJ21" s="389"/>
+      <c r="AK21" s="389"/>
+      <c r="AL21" s="389"/>
+      <c r="AM21" s="389"/>
+      <c r="AN21" s="389"/>
+      <c r="AO21" s="389"/>
+      <c r="AP21" s="389"/>
+      <c r="AQ21" s="389"/>
+      <c r="AR21" s="389"/>
+      <c r="AS21" s="389"/>
+      <c r="AT21" s="393" t="s">
         <v>12</v>
       </c>
-      <c r="AU21" s="396"/>
-      <c r="AV21" s="396"/>
-      <c r="AW21" s="396"/>
-      <c r="AX21" s="396"/>
-      <c r="AY21" s="397"/>
+      <c r="AU21" s="393"/>
+      <c r="AV21" s="393"/>
+      <c r="AW21" s="393"/>
+      <c r="AX21" s="393"/>
+      <c r="AY21" s="394"/>
       <c r="AZ21" s="20"/>
       <c r="BA21" s="20"/>
-      <c r="BD21" s="412"/>
-      <c r="BE21" s="413"/>
-      <c r="BF21" s="413"/>
-      <c r="BG21" s="413"/>
-      <c r="BH21" s="413"/>
-      <c r="BI21" s="413"/>
-      <c r="BJ21" s="413"/>
-      <c r="BK21" s="413"/>
-      <c r="BL21" s="413"/>
-      <c r="BM21" s="413"/>
-      <c r="BN21" s="413"/>
-      <c r="BO21" s="413"/>
-      <c r="BP21" s="413"/>
-      <c r="BQ21" s="413"/>
-      <c r="BR21" s="413"/>
-      <c r="BS21" s="413"/>
-      <c r="BT21" s="413"/>
-      <c r="BU21" s="414"/>
+      <c r="BD21" s="409"/>
+      <c r="BE21" s="410"/>
+      <c r="BF21" s="410"/>
+      <c r="BG21" s="410"/>
+      <c r="BH21" s="410"/>
+      <c r="BI21" s="410"/>
+      <c r="BJ21" s="410"/>
+      <c r="BK21" s="410"/>
+      <c r="BL21" s="410"/>
+      <c r="BM21" s="410"/>
+      <c r="BN21" s="410"/>
+      <c r="BO21" s="410"/>
+      <c r="BP21" s="410"/>
+      <c r="BQ21" s="410"/>
+      <c r="BR21" s="410"/>
+      <c r="BS21" s="410"/>
+      <c r="BT21" s="410"/>
+      <c r="BU21" s="411"/>
       <c r="BV21" s="24"/>
       <c r="BW21" s="24"/>
       <c r="BX21" s="24"/>
@@ -14628,60 +14627,60 @@
       <c r="E22" s="386"/>
       <c r="F22" s="386"/>
       <c r="G22" s="387"/>
-      <c r="H22" s="391"/>
-      <c r="I22" s="392"/>
-      <c r="J22" s="392"/>
-      <c r="K22" s="392"/>
-      <c r="L22" s="392"/>
-      <c r="M22" s="392"/>
-      <c r="N22" s="392"/>
-      <c r="O22" s="392"/>
-      <c r="P22" s="392"/>
-      <c r="Q22" s="392"/>
-      <c r="R22" s="392"/>
-      <c r="S22" s="392"/>
-      <c r="T22" s="392"/>
-      <c r="U22" s="392"/>
-      <c r="V22" s="392"/>
-      <c r="W22" s="392"/>
-      <c r="X22" s="392"/>
-      <c r="Y22" s="392"/>
-      <c r="Z22" s="392"/>
-      <c r="AA22" s="392"/>
-      <c r="AB22" s="392"/>
-      <c r="AC22" s="392"/>
-      <c r="AD22" s="392"/>
-      <c r="AE22" s="392"/>
-      <c r="AF22" s="392"/>
-      <c r="AG22" s="392"/>
-      <c r="AH22" s="392"/>
-      <c r="AI22" s="392"/>
-      <c r="AJ22" s="392"/>
-      <c r="AK22" s="392"/>
-      <c r="AL22" s="392"/>
-      <c r="AM22" s="392"/>
-      <c r="AN22" s="392"/>
-      <c r="AO22" s="392"/>
-      <c r="AP22" s="392"/>
-      <c r="AQ22" s="392"/>
-      <c r="AR22" s="392"/>
-      <c r="AS22" s="392"/>
-      <c r="AT22" s="396"/>
-      <c r="AU22" s="396"/>
-      <c r="AV22" s="396"/>
-      <c r="AW22" s="396"/>
-      <c r="AX22" s="396"/>
-      <c r="AY22" s="397"/>
+      <c r="H22" s="388"/>
+      <c r="I22" s="389"/>
+      <c r="J22" s="389"/>
+      <c r="K22" s="389"/>
+      <c r="L22" s="389"/>
+      <c r="M22" s="389"/>
+      <c r="N22" s="389"/>
+      <c r="O22" s="389"/>
+      <c r="P22" s="389"/>
+      <c r="Q22" s="389"/>
+      <c r="R22" s="389"/>
+      <c r="S22" s="389"/>
+      <c r="T22" s="389"/>
+      <c r="U22" s="389"/>
+      <c r="V22" s="389"/>
+      <c r="W22" s="389"/>
+      <c r="X22" s="389"/>
+      <c r="Y22" s="389"/>
+      <c r="Z22" s="389"/>
+      <c r="AA22" s="389"/>
+      <c r="AB22" s="389"/>
+      <c r="AC22" s="389"/>
+      <c r="AD22" s="389"/>
+      <c r="AE22" s="389"/>
+      <c r="AF22" s="389"/>
+      <c r="AG22" s="389"/>
+      <c r="AH22" s="389"/>
+      <c r="AI22" s="389"/>
+      <c r="AJ22" s="389"/>
+      <c r="AK22" s="389"/>
+      <c r="AL22" s="389"/>
+      <c r="AM22" s="389"/>
+      <c r="AN22" s="389"/>
+      <c r="AO22" s="389"/>
+      <c r="AP22" s="389"/>
+      <c r="AQ22" s="389"/>
+      <c r="AR22" s="389"/>
+      <c r="AS22" s="389"/>
+      <c r="AT22" s="393"/>
+      <c r="AU22" s="393"/>
+      <c r="AV22" s="393"/>
+      <c r="AW22" s="393"/>
+      <c r="AX22" s="393"/>
+      <c r="AY22" s="394"/>
       <c r="AZ22" s="26"/>
       <c r="BA22" s="26"/>
-      <c r="BD22" s="405" t="s">
+      <c r="BD22" s="402" t="s">
         <v>90</v>
       </c>
-      <c r="BE22" s="406"/>
-      <c r="BF22" s="406"/>
-      <c r="BG22" s="406"/>
-      <c r="BH22" s="406"/>
-      <c r="BI22" s="406"/>
+      <c r="BE22" s="403"/>
+      <c r="BF22" s="403"/>
+      <c r="BG22" s="403"/>
+      <c r="BH22" s="403"/>
+      <c r="BI22" s="403"/>
       <c r="BJ22" s="27"/>
       <c r="BK22" s="27"/>
       <c r="BL22" s="27"/>
@@ -14725,53 +14724,53 @@
       <c r="E23" s="386"/>
       <c r="F23" s="386"/>
       <c r="G23" s="387"/>
-      <c r="H23" s="391"/>
-      <c r="I23" s="392"/>
-      <c r="J23" s="392"/>
-      <c r="K23" s="392"/>
-      <c r="L23" s="392"/>
-      <c r="M23" s="392"/>
-      <c r="N23" s="392"/>
-      <c r="O23" s="392"/>
-      <c r="P23" s="392"/>
-      <c r="Q23" s="392"/>
-      <c r="R23" s="392"/>
-      <c r="S23" s="392"/>
-      <c r="T23" s="392"/>
-      <c r="U23" s="392"/>
-      <c r="V23" s="392"/>
-      <c r="W23" s="392"/>
-      <c r="X23" s="392"/>
-      <c r="Y23" s="392"/>
-      <c r="Z23" s="392"/>
-      <c r="AA23" s="392"/>
-      <c r="AB23" s="392"/>
-      <c r="AC23" s="392"/>
-      <c r="AD23" s="392"/>
-      <c r="AE23" s="392"/>
-      <c r="AF23" s="392"/>
-      <c r="AG23" s="392"/>
-      <c r="AH23" s="392"/>
-      <c r="AI23" s="392"/>
-      <c r="AJ23" s="392"/>
-      <c r="AK23" s="392"/>
-      <c r="AL23" s="392"/>
-      <c r="AM23" s="392"/>
-      <c r="AN23" s="392"/>
-      <c r="AO23" s="392"/>
-      <c r="AP23" s="392"/>
-      <c r="AQ23" s="392"/>
-      <c r="AR23" s="392"/>
-      <c r="AS23" s="392"/>
-      <c r="AT23" s="396"/>
-      <c r="AU23" s="396"/>
-      <c r="AV23" s="396"/>
-      <c r="AW23" s="396"/>
-      <c r="AX23" s="396"/>
-      <c r="AY23" s="397"/>
+      <c r="H23" s="388"/>
+      <c r="I23" s="389"/>
+      <c r="J23" s="389"/>
+      <c r="K23" s="389"/>
+      <c r="L23" s="389"/>
+      <c r="M23" s="389"/>
+      <c r="N23" s="389"/>
+      <c r="O23" s="389"/>
+      <c r="P23" s="389"/>
+      <c r="Q23" s="389"/>
+      <c r="R23" s="389"/>
+      <c r="S23" s="389"/>
+      <c r="T23" s="389"/>
+      <c r="U23" s="389"/>
+      <c r="V23" s="389"/>
+      <c r="W23" s="389"/>
+      <c r="X23" s="389"/>
+      <c r="Y23" s="389"/>
+      <c r="Z23" s="389"/>
+      <c r="AA23" s="389"/>
+      <c r="AB23" s="389"/>
+      <c r="AC23" s="389"/>
+      <c r="AD23" s="389"/>
+      <c r="AE23" s="389"/>
+      <c r="AF23" s="389"/>
+      <c r="AG23" s="389"/>
+      <c r="AH23" s="389"/>
+      <c r="AI23" s="389"/>
+      <c r="AJ23" s="389"/>
+      <c r="AK23" s="389"/>
+      <c r="AL23" s="389"/>
+      <c r="AM23" s="389"/>
+      <c r="AN23" s="389"/>
+      <c r="AO23" s="389"/>
+      <c r="AP23" s="389"/>
+      <c r="AQ23" s="389"/>
+      <c r="AR23" s="389"/>
+      <c r="AS23" s="389"/>
+      <c r="AT23" s="393"/>
+      <c r="AU23" s="393"/>
+      <c r="AV23" s="393"/>
+      <c r="AW23" s="393"/>
+      <c r="AX23" s="393"/>
+      <c r="AY23" s="394"/>
       <c r="AZ23" s="26"/>
       <c r="BA23" s="26"/>
-      <c r="BD23" s="415"/>
+      <c r="BD23" s="412"/>
       <c r="BE23" s="383"/>
       <c r="BF23" s="383"/>
       <c r="BG23" s="383"/>
@@ -14822,53 +14821,53 @@
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="31"/>
-      <c r="H24" s="391"/>
-      <c r="I24" s="392"/>
-      <c r="J24" s="392"/>
-      <c r="K24" s="392"/>
-      <c r="L24" s="392"/>
-      <c r="M24" s="392"/>
-      <c r="N24" s="392"/>
-      <c r="O24" s="392"/>
-      <c r="P24" s="392"/>
-      <c r="Q24" s="392"/>
-      <c r="R24" s="392"/>
-      <c r="S24" s="392"/>
-      <c r="T24" s="392"/>
-      <c r="U24" s="392"/>
-      <c r="V24" s="392"/>
-      <c r="W24" s="392"/>
-      <c r="X24" s="392"/>
-      <c r="Y24" s="392"/>
-      <c r="Z24" s="392"/>
-      <c r="AA24" s="392"/>
-      <c r="AB24" s="392"/>
-      <c r="AC24" s="392"/>
-      <c r="AD24" s="392"/>
-      <c r="AE24" s="392"/>
-      <c r="AF24" s="392"/>
-      <c r="AG24" s="392"/>
-      <c r="AH24" s="392"/>
-      <c r="AI24" s="392"/>
-      <c r="AJ24" s="392"/>
-      <c r="AK24" s="392"/>
-      <c r="AL24" s="392"/>
-      <c r="AM24" s="392"/>
-      <c r="AN24" s="392"/>
-      <c r="AO24" s="392"/>
-      <c r="AP24" s="392"/>
-      <c r="AQ24" s="392"/>
-      <c r="AR24" s="392"/>
-      <c r="AS24" s="392"/>
-      <c r="AT24" s="396"/>
-      <c r="AU24" s="396"/>
-      <c r="AV24" s="396"/>
-      <c r="AW24" s="396"/>
-      <c r="AX24" s="396"/>
-      <c r="AY24" s="397"/>
+      <c r="H24" s="388"/>
+      <c r="I24" s="389"/>
+      <c r="J24" s="389"/>
+      <c r="K24" s="389"/>
+      <c r="L24" s="389"/>
+      <c r="M24" s="389"/>
+      <c r="N24" s="389"/>
+      <c r="O24" s="389"/>
+      <c r="P24" s="389"/>
+      <c r="Q24" s="389"/>
+      <c r="R24" s="389"/>
+      <c r="S24" s="389"/>
+      <c r="T24" s="389"/>
+      <c r="U24" s="389"/>
+      <c r="V24" s="389"/>
+      <c r="W24" s="389"/>
+      <c r="X24" s="389"/>
+      <c r="Y24" s="389"/>
+      <c r="Z24" s="389"/>
+      <c r="AA24" s="389"/>
+      <c r="AB24" s="389"/>
+      <c r="AC24" s="389"/>
+      <c r="AD24" s="389"/>
+      <c r="AE24" s="389"/>
+      <c r="AF24" s="389"/>
+      <c r="AG24" s="389"/>
+      <c r="AH24" s="389"/>
+      <c r="AI24" s="389"/>
+      <c r="AJ24" s="389"/>
+      <c r="AK24" s="389"/>
+      <c r="AL24" s="389"/>
+      <c r="AM24" s="389"/>
+      <c r="AN24" s="389"/>
+      <c r="AO24" s="389"/>
+      <c r="AP24" s="389"/>
+      <c r="AQ24" s="389"/>
+      <c r="AR24" s="389"/>
+      <c r="AS24" s="389"/>
+      <c r="AT24" s="393"/>
+      <c r="AU24" s="393"/>
+      <c r="AV24" s="393"/>
+      <c r="AW24" s="393"/>
+      <c r="AX24" s="393"/>
+      <c r="AY24" s="394"/>
       <c r="AZ24" s="26"/>
       <c r="BA24" s="26"/>
-      <c r="BD24" s="415"/>
+      <c r="BD24" s="412"/>
       <c r="BE24" s="383"/>
       <c r="BF24" s="383"/>
       <c r="BG24" s="383"/>
@@ -14948,20 +14947,20 @@
       <c r="AF25" s="358"/>
       <c r="AG25" s="358"/>
       <c r="AH25" s="358"/>
-      <c r="AI25" s="398" t="s">
+      <c r="AI25" s="395" t="s">
         <v>27</v>
       </c>
-      <c r="AJ25" s="398"/>
-      <c r="AK25" s="394"/>
-      <c r="AL25" s="394"/>
-      <c r="AM25" s="394"/>
-      <c r="AN25" s="394"/>
-      <c r="AO25" s="394"/>
-      <c r="AP25" s="394"/>
-      <c r="AQ25" s="394"/>
-      <c r="AR25" s="394"/>
-      <c r="AS25" s="394"/>
-      <c r="AT25" s="394"/>
+      <c r="AJ25" s="395"/>
+      <c r="AK25" s="391"/>
+      <c r="AL25" s="391"/>
+      <c r="AM25" s="391"/>
+      <c r="AN25" s="391"/>
+      <c r="AO25" s="391"/>
+      <c r="AP25" s="391"/>
+      <c r="AQ25" s="391"/>
+      <c r="AR25" s="391"/>
+      <c r="AS25" s="391"/>
+      <c r="AT25" s="391"/>
       <c r="AU25" s="34"/>
       <c r="AV25" s="35"/>
       <c r="AW25" s="35"/>
@@ -14969,7 +14968,7 @@
       <c r="AY25" s="37"/>
       <c r="AZ25" s="36"/>
       <c r="BA25" s="36"/>
-      <c r="BD25" s="415"/>
+      <c r="BD25" s="412"/>
       <c r="BE25" s="383"/>
       <c r="BF25" s="383"/>
       <c r="BG25" s="383"/>
@@ -15045,18 +15044,18 @@
       <c r="AF26" s="361"/>
       <c r="AG26" s="361"/>
       <c r="AH26" s="361"/>
-      <c r="AI26" s="399"/>
-      <c r="AJ26" s="399"/>
-      <c r="AK26" s="395"/>
-      <c r="AL26" s="395"/>
-      <c r="AM26" s="395"/>
-      <c r="AN26" s="395"/>
-      <c r="AO26" s="395"/>
-      <c r="AP26" s="395"/>
-      <c r="AQ26" s="395"/>
-      <c r="AR26" s="395"/>
-      <c r="AS26" s="395"/>
-      <c r="AT26" s="395"/>
+      <c r="AI26" s="396"/>
+      <c r="AJ26" s="396"/>
+      <c r="AK26" s="392"/>
+      <c r="AL26" s="392"/>
+      <c r="AM26" s="392"/>
+      <c r="AN26" s="392"/>
+      <c r="AO26" s="392"/>
+      <c r="AP26" s="392"/>
+      <c r="AQ26" s="392"/>
+      <c r="AR26" s="392"/>
+      <c r="AS26" s="392"/>
+      <c r="AT26" s="392"/>
       <c r="AU26" s="40"/>
       <c r="AV26" s="40"/>
       <c r="AW26" s="40"/>
@@ -16846,27 +16845,27 @@
         <v>81</v>
       </c>
       <c r="BX44" s="320"/>
-      <c r="BY44" s="418" t="s">
+      <c r="BY44" s="415" t="s">
         <v>83</v>
       </c>
-      <c r="BZ44" s="418"/>
-      <c r="CA44" s="418"/>
-      <c r="CB44" s="418"/>
-      <c r="CC44" s="418"/>
-      <c r="CD44" s="418"/>
-      <c r="CE44" s="418"/>
-      <c r="CF44" s="418"/>
-      <c r="CG44" s="418"/>
-      <c r="CH44" s="418"/>
-      <c r="CI44" s="418"/>
-      <c r="CJ44" s="418"/>
-      <c r="CK44" s="418"/>
-      <c r="CL44" s="418"/>
-      <c r="CM44" s="418"/>
-      <c r="CN44" s="418"/>
-      <c r="CO44" s="418"/>
-      <c r="CP44" s="418"/>
-      <c r="CQ44" s="418"/>
+      <c r="BZ44" s="415"/>
+      <c r="CA44" s="415"/>
+      <c r="CB44" s="415"/>
+      <c r="CC44" s="415"/>
+      <c r="CD44" s="415"/>
+      <c r="CE44" s="415"/>
+      <c r="CF44" s="415"/>
+      <c r="CG44" s="415"/>
+      <c r="CH44" s="415"/>
+      <c r="CI44" s="415"/>
+      <c r="CJ44" s="415"/>
+      <c r="CK44" s="415"/>
+      <c r="CL44" s="415"/>
+      <c r="CM44" s="415"/>
+      <c r="CN44" s="415"/>
+      <c r="CO44" s="415"/>
+      <c r="CP44" s="415"/>
+      <c r="CQ44" s="415"/>
       <c r="CR44" s="80"/>
       <c r="CS44" s="81"/>
       <c r="CT44" s="70"/>
@@ -16949,25 +16948,25 @@
       <c r="BV45" s="82"/>
       <c r="BW45" s="321"/>
       <c r="BX45" s="321"/>
-      <c r="BY45" s="419"/>
-      <c r="BZ45" s="419"/>
-      <c r="CA45" s="419"/>
-      <c r="CB45" s="419"/>
-      <c r="CC45" s="419"/>
-      <c r="CD45" s="419"/>
-      <c r="CE45" s="419"/>
-      <c r="CF45" s="419"/>
-      <c r="CG45" s="419"/>
-      <c r="CH45" s="419"/>
-      <c r="CI45" s="419"/>
-      <c r="CJ45" s="419"/>
-      <c r="CK45" s="419"/>
-      <c r="CL45" s="419"/>
-      <c r="CM45" s="419"/>
-      <c r="CN45" s="419"/>
-      <c r="CO45" s="419"/>
-      <c r="CP45" s="419"/>
-      <c r="CQ45" s="419"/>
+      <c r="BY45" s="416"/>
+      <c r="BZ45" s="416"/>
+      <c r="CA45" s="416"/>
+      <c r="CB45" s="416"/>
+      <c r="CC45" s="416"/>
+      <c r="CD45" s="416"/>
+      <c r="CE45" s="416"/>
+      <c r="CF45" s="416"/>
+      <c r="CG45" s="416"/>
+      <c r="CH45" s="416"/>
+      <c r="CI45" s="416"/>
+      <c r="CJ45" s="416"/>
+      <c r="CK45" s="416"/>
+      <c r="CL45" s="416"/>
+      <c r="CM45" s="416"/>
+      <c r="CN45" s="416"/>
+      <c r="CO45" s="416"/>
+      <c r="CP45" s="416"/>
+      <c r="CQ45" s="416"/>
       <c r="CR45" s="83"/>
       <c r="CS45" s="84"/>
     </row>
@@ -17051,31 +17050,31 @@
       <c r="BT46" s="58"/>
       <c r="BU46" s="58"/>
       <c r="BV46" s="82"/>
-      <c r="BW46" s="417" t="s">
+      <c r="BW46" s="414" t="s">
         <v>80</v>
       </c>
-      <c r="BX46" s="417"/>
-      <c r="BY46" s="417"/>
-      <c r="BZ46" s="417"/>
-      <c r="CA46" s="417"/>
-      <c r="CB46" s="417"/>
-      <c r="CC46" s="417"/>
-      <c r="CD46" s="417"/>
-      <c r="CE46" s="417"/>
-      <c r="CF46" s="417"/>
-      <c r="CG46" s="417"/>
-      <c r="CH46" s="417"/>
-      <c r="CI46" s="417"/>
-      <c r="CJ46" s="417"/>
-      <c r="CK46" s="417"/>
-      <c r="CL46" s="417"/>
-      <c r="CM46" s="417"/>
-      <c r="CN46" s="417"/>
-      <c r="CO46" s="417"/>
-      <c r="CP46" s="417"/>
-      <c r="CQ46" s="417"/>
-      <c r="CR46" s="417"/>
-      <c r="CS46" s="420"/>
+      <c r="BX46" s="414"/>
+      <c r="BY46" s="414"/>
+      <c r="BZ46" s="414"/>
+      <c r="CA46" s="414"/>
+      <c r="CB46" s="414"/>
+      <c r="CC46" s="414"/>
+      <c r="CD46" s="414"/>
+      <c r="CE46" s="414"/>
+      <c r="CF46" s="414"/>
+      <c r="CG46" s="414"/>
+      <c r="CH46" s="414"/>
+      <c r="CI46" s="414"/>
+      <c r="CJ46" s="414"/>
+      <c r="CK46" s="414"/>
+      <c r="CL46" s="414"/>
+      <c r="CM46" s="414"/>
+      <c r="CN46" s="414"/>
+      <c r="CO46" s="414"/>
+      <c r="CP46" s="414"/>
+      <c r="CQ46" s="414"/>
+      <c r="CR46" s="414"/>
+      <c r="CS46" s="417"/>
       <c r="CX46" s="8"/>
       <c r="CY46" s="8"/>
       <c r="CZ46" s="8"/>
@@ -17196,28 +17195,28 @@
       <c r="BT47" s="168"/>
       <c r="BU47" s="168"/>
       <c r="BV47" s="94"/>
-      <c r="BW47" s="421"/>
-      <c r="BX47" s="421"/>
-      <c r="BY47" s="421"/>
-      <c r="BZ47" s="421"/>
-      <c r="CA47" s="421"/>
-      <c r="CB47" s="421"/>
-      <c r="CC47" s="421"/>
-      <c r="CD47" s="421"/>
-      <c r="CE47" s="421"/>
-      <c r="CF47" s="421"/>
-      <c r="CG47" s="421"/>
-      <c r="CH47" s="421"/>
-      <c r="CI47" s="421"/>
-      <c r="CJ47" s="421"/>
-      <c r="CK47" s="421"/>
-      <c r="CL47" s="421"/>
-      <c r="CM47" s="421"/>
-      <c r="CN47" s="421"/>
-      <c r="CO47" s="421"/>
-      <c r="CP47" s="421"/>
-      <c r="CQ47" s="421"/>
-      <c r="CR47" s="421"/>
+      <c r="BW47" s="418"/>
+      <c r="BX47" s="418"/>
+      <c r="BY47" s="418"/>
+      <c r="BZ47" s="418"/>
+      <c r="CA47" s="418"/>
+      <c r="CB47" s="418"/>
+      <c r="CC47" s="418"/>
+      <c r="CD47" s="418"/>
+      <c r="CE47" s="418"/>
+      <c r="CF47" s="418"/>
+      <c r="CG47" s="418"/>
+      <c r="CH47" s="418"/>
+      <c r="CI47" s="418"/>
+      <c r="CJ47" s="418"/>
+      <c r="CK47" s="418"/>
+      <c r="CL47" s="418"/>
+      <c r="CM47" s="418"/>
+      <c r="CN47" s="418"/>
+      <c r="CO47" s="418"/>
+      <c r="CP47" s="418"/>
+      <c r="CQ47" s="418"/>
+      <c r="CR47" s="418"/>
       <c r="CS47" s="178"/>
       <c r="CX47" s="95"/>
       <c r="CY47" s="95"/>
@@ -19696,27 +19695,27 @@
         <v>81</v>
       </c>
       <c r="BX69" s="319"/>
-      <c r="BY69" s="418" t="s">
+      <c r="BY69" s="415" t="s">
         <v>83</v>
       </c>
-      <c r="BZ69" s="418"/>
-      <c r="CA69" s="418"/>
-      <c r="CB69" s="418"/>
-      <c r="CC69" s="418"/>
-      <c r="CD69" s="418"/>
-      <c r="CE69" s="418"/>
-      <c r="CF69" s="418"/>
-      <c r="CG69" s="418"/>
-      <c r="CH69" s="418"/>
-      <c r="CI69" s="418"/>
-      <c r="CJ69" s="418"/>
-      <c r="CK69" s="418"/>
-      <c r="CL69" s="418"/>
-      <c r="CM69" s="418"/>
-      <c r="CN69" s="418"/>
-      <c r="CO69" s="418"/>
-      <c r="CP69" s="418"/>
-      <c r="CQ69" s="418"/>
+      <c r="BZ69" s="415"/>
+      <c r="CA69" s="415"/>
+      <c r="CB69" s="415"/>
+      <c r="CC69" s="415"/>
+      <c r="CD69" s="415"/>
+      <c r="CE69" s="415"/>
+      <c r="CF69" s="415"/>
+      <c r="CG69" s="415"/>
+      <c r="CH69" s="415"/>
+      <c r="CI69" s="415"/>
+      <c r="CJ69" s="415"/>
+      <c r="CK69" s="415"/>
+      <c r="CL69" s="415"/>
+      <c r="CM69" s="415"/>
+      <c r="CN69" s="415"/>
+      <c r="CO69" s="415"/>
+      <c r="CP69" s="415"/>
+      <c r="CQ69" s="415"/>
       <c r="CR69" s="80"/>
       <c r="CS69" s="81"/>
       <c r="DI69" s="114"/>
@@ -19797,27 +19796,27 @@
       <c r="BT70" s="58"/>
       <c r="BU70" s="58"/>
       <c r="BV70" s="82"/>
-      <c r="BW70" s="422"/>
-      <c r="BX70" s="422"/>
-      <c r="BY70" s="419"/>
-      <c r="BZ70" s="419"/>
-      <c r="CA70" s="419"/>
-      <c r="CB70" s="419"/>
-      <c r="CC70" s="419"/>
-      <c r="CD70" s="419"/>
-      <c r="CE70" s="419"/>
-      <c r="CF70" s="419"/>
-      <c r="CG70" s="419"/>
-      <c r="CH70" s="419"/>
-      <c r="CI70" s="419"/>
-      <c r="CJ70" s="419"/>
-      <c r="CK70" s="419"/>
-      <c r="CL70" s="419"/>
-      <c r="CM70" s="419"/>
-      <c r="CN70" s="419"/>
-      <c r="CO70" s="419"/>
-      <c r="CP70" s="419"/>
-      <c r="CQ70" s="419"/>
+      <c r="BW70" s="419"/>
+      <c r="BX70" s="419"/>
+      <c r="BY70" s="416"/>
+      <c r="BZ70" s="416"/>
+      <c r="CA70" s="416"/>
+      <c r="CB70" s="416"/>
+      <c r="CC70" s="416"/>
+      <c r="CD70" s="416"/>
+      <c r="CE70" s="416"/>
+      <c r="CF70" s="416"/>
+      <c r="CG70" s="416"/>
+      <c r="CH70" s="416"/>
+      <c r="CI70" s="416"/>
+      <c r="CJ70" s="416"/>
+      <c r="CK70" s="416"/>
+      <c r="CL70" s="416"/>
+      <c r="CM70" s="416"/>
+      <c r="CN70" s="416"/>
+      <c r="CO70" s="416"/>
+      <c r="CP70" s="416"/>
+      <c r="CQ70" s="416"/>
       <c r="CR70" s="83"/>
       <c r="CS70" s="84"/>
     </row>
@@ -19903,31 +19902,31 @@
       <c r="BT71" s="58"/>
       <c r="BU71" s="58"/>
       <c r="BV71" s="82"/>
-      <c r="BW71" s="417" t="s">
+      <c r="BW71" s="414" t="s">
         <v>80</v>
       </c>
-      <c r="BX71" s="417"/>
-      <c r="BY71" s="417"/>
-      <c r="BZ71" s="417"/>
-      <c r="CA71" s="417"/>
-      <c r="CB71" s="417"/>
-      <c r="CC71" s="417"/>
-      <c r="CD71" s="417"/>
-      <c r="CE71" s="417"/>
-      <c r="CF71" s="417"/>
-      <c r="CG71" s="417"/>
-      <c r="CH71" s="417"/>
-      <c r="CI71" s="417"/>
-      <c r="CJ71" s="417"/>
-      <c r="CK71" s="417"/>
-      <c r="CL71" s="417"/>
-      <c r="CM71" s="417"/>
-      <c r="CN71" s="417"/>
-      <c r="CO71" s="417"/>
-      <c r="CP71" s="417"/>
-      <c r="CQ71" s="417"/>
-      <c r="CR71" s="417"/>
-      <c r="CS71" s="420"/>
+      <c r="BX71" s="414"/>
+      <c r="BY71" s="414"/>
+      <c r="BZ71" s="414"/>
+      <c r="CA71" s="414"/>
+      <c r="CB71" s="414"/>
+      <c r="CC71" s="414"/>
+      <c r="CD71" s="414"/>
+      <c r="CE71" s="414"/>
+      <c r="CF71" s="414"/>
+      <c r="CG71" s="414"/>
+      <c r="CH71" s="414"/>
+      <c r="CI71" s="414"/>
+      <c r="CJ71" s="414"/>
+      <c r="CK71" s="414"/>
+      <c r="CL71" s="414"/>
+      <c r="CM71" s="414"/>
+      <c r="CN71" s="414"/>
+      <c r="CO71" s="414"/>
+      <c r="CP71" s="414"/>
+      <c r="CQ71" s="414"/>
+      <c r="CR71" s="414"/>
+      <c r="CS71" s="417"/>
     </row>
     <row r="72" spans="1:113" ht="10.5" customHeight="1">
       <c r="A72" s="126"/>
@@ -20007,28 +20006,28 @@
       <c r="BT72" s="168"/>
       <c r="BU72" s="168"/>
       <c r="BV72" s="94"/>
-      <c r="BW72" s="421"/>
-      <c r="BX72" s="421"/>
-      <c r="BY72" s="421"/>
-      <c r="BZ72" s="421"/>
-      <c r="CA72" s="421"/>
-      <c r="CB72" s="421"/>
-      <c r="CC72" s="421"/>
-      <c r="CD72" s="421"/>
-      <c r="CE72" s="421"/>
-      <c r="CF72" s="421"/>
-      <c r="CG72" s="421"/>
-      <c r="CH72" s="421"/>
-      <c r="CI72" s="421"/>
-      <c r="CJ72" s="421"/>
-      <c r="CK72" s="421"/>
-      <c r="CL72" s="421"/>
-      <c r="CM72" s="421"/>
-      <c r="CN72" s="421"/>
-      <c r="CO72" s="421"/>
-      <c r="CP72" s="421"/>
-      <c r="CQ72" s="421"/>
-      <c r="CR72" s="421"/>
+      <c r="BW72" s="418"/>
+      <c r="BX72" s="418"/>
+      <c r="BY72" s="418"/>
+      <c r="BZ72" s="418"/>
+      <c r="CA72" s="418"/>
+      <c r="CB72" s="418"/>
+      <c r="CC72" s="418"/>
+      <c r="CD72" s="418"/>
+      <c r="CE72" s="418"/>
+      <c r="CF72" s="418"/>
+      <c r="CG72" s="418"/>
+      <c r="CH72" s="418"/>
+      <c r="CI72" s="418"/>
+      <c r="CJ72" s="418"/>
+      <c r="CK72" s="418"/>
+      <c r="CL72" s="418"/>
+      <c r="CM72" s="418"/>
+      <c r="CN72" s="418"/>
+      <c r="CO72" s="418"/>
+      <c r="CP72" s="418"/>
+      <c r="CQ72" s="418"/>
+      <c r="CR72" s="418"/>
       <c r="CS72" s="178"/>
     </row>
     <row r="73" spans="1:113" ht="10.5" customHeight="1">
@@ -22164,27 +22163,27 @@
         <v>81</v>
       </c>
       <c r="BX94" s="319"/>
-      <c r="BY94" s="418" t="s">
+      <c r="BY94" s="415" t="s">
         <v>83</v>
       </c>
-      <c r="BZ94" s="418"/>
-      <c r="CA94" s="418"/>
-      <c r="CB94" s="418"/>
-      <c r="CC94" s="418"/>
-      <c r="CD94" s="418"/>
-      <c r="CE94" s="418"/>
-      <c r="CF94" s="418"/>
-      <c r="CG94" s="418"/>
-      <c r="CH94" s="418"/>
-      <c r="CI94" s="418"/>
-      <c r="CJ94" s="418"/>
-      <c r="CK94" s="418"/>
-      <c r="CL94" s="418"/>
-      <c r="CM94" s="418"/>
-      <c r="CN94" s="418"/>
-      <c r="CO94" s="418"/>
-      <c r="CP94" s="418"/>
-      <c r="CQ94" s="418"/>
+      <c r="BZ94" s="415"/>
+      <c r="CA94" s="415"/>
+      <c r="CB94" s="415"/>
+      <c r="CC94" s="415"/>
+      <c r="CD94" s="415"/>
+      <c r="CE94" s="415"/>
+      <c r="CF94" s="415"/>
+      <c r="CG94" s="415"/>
+      <c r="CH94" s="415"/>
+      <c r="CI94" s="415"/>
+      <c r="CJ94" s="415"/>
+      <c r="CK94" s="415"/>
+      <c r="CL94" s="415"/>
+      <c r="CM94" s="415"/>
+      <c r="CN94" s="415"/>
+      <c r="CO94" s="415"/>
+      <c r="CP94" s="415"/>
+      <c r="CQ94" s="415"/>
       <c r="CR94" s="80"/>
       <c r="CS94" s="81"/>
       <c r="DI94" s="114"/>
@@ -22265,27 +22264,27 @@
       <c r="BT95" s="58"/>
       <c r="BU95" s="58"/>
       <c r="BV95" s="82"/>
-      <c r="BW95" s="422"/>
-      <c r="BX95" s="422"/>
-      <c r="BY95" s="419"/>
-      <c r="BZ95" s="419"/>
-      <c r="CA95" s="419"/>
-      <c r="CB95" s="419"/>
-      <c r="CC95" s="419"/>
-      <c r="CD95" s="419"/>
-      <c r="CE95" s="419"/>
-      <c r="CF95" s="419"/>
-      <c r="CG95" s="419"/>
-      <c r="CH95" s="419"/>
-      <c r="CI95" s="419"/>
-      <c r="CJ95" s="419"/>
-      <c r="CK95" s="419"/>
-      <c r="CL95" s="419"/>
-      <c r="CM95" s="419"/>
-      <c r="CN95" s="419"/>
-      <c r="CO95" s="419"/>
-      <c r="CP95" s="419"/>
-      <c r="CQ95" s="419"/>
+      <c r="BW95" s="419"/>
+      <c r="BX95" s="419"/>
+      <c r="BY95" s="416"/>
+      <c r="BZ95" s="416"/>
+      <c r="CA95" s="416"/>
+      <c r="CB95" s="416"/>
+      <c r="CC95" s="416"/>
+      <c r="CD95" s="416"/>
+      <c r="CE95" s="416"/>
+      <c r="CF95" s="416"/>
+      <c r="CG95" s="416"/>
+      <c r="CH95" s="416"/>
+      <c r="CI95" s="416"/>
+      <c r="CJ95" s="416"/>
+      <c r="CK95" s="416"/>
+      <c r="CL95" s="416"/>
+      <c r="CM95" s="416"/>
+      <c r="CN95" s="416"/>
+      <c r="CO95" s="416"/>
+      <c r="CP95" s="416"/>
+      <c r="CQ95" s="416"/>
       <c r="CR95" s="83"/>
       <c r="CS95" s="84"/>
     </row>
@@ -22369,31 +22368,31 @@
       <c r="BT96" s="58"/>
       <c r="BU96" s="58"/>
       <c r="BV96" s="82"/>
-      <c r="BW96" s="417" t="s">
+      <c r="BW96" s="414" t="s">
         <v>80</v>
       </c>
-      <c r="BX96" s="417"/>
-      <c r="BY96" s="417"/>
-      <c r="BZ96" s="417"/>
-      <c r="CA96" s="417"/>
-      <c r="CB96" s="417"/>
-      <c r="CC96" s="417"/>
-      <c r="CD96" s="417"/>
-      <c r="CE96" s="417"/>
-      <c r="CF96" s="417"/>
-      <c r="CG96" s="417"/>
-      <c r="CH96" s="417"/>
-      <c r="CI96" s="417"/>
-      <c r="CJ96" s="417"/>
-      <c r="CK96" s="417"/>
-      <c r="CL96" s="417"/>
-      <c r="CM96" s="417"/>
-      <c r="CN96" s="417"/>
-      <c r="CO96" s="417"/>
-      <c r="CP96" s="417"/>
-      <c r="CQ96" s="417"/>
-      <c r="CR96" s="417"/>
-      <c r="CS96" s="420"/>
+      <c r="BX96" s="414"/>
+      <c r="BY96" s="414"/>
+      <c r="BZ96" s="414"/>
+      <c r="CA96" s="414"/>
+      <c r="CB96" s="414"/>
+      <c r="CC96" s="414"/>
+      <c r="CD96" s="414"/>
+      <c r="CE96" s="414"/>
+      <c r="CF96" s="414"/>
+      <c r="CG96" s="414"/>
+      <c r="CH96" s="414"/>
+      <c r="CI96" s="414"/>
+      <c r="CJ96" s="414"/>
+      <c r="CK96" s="414"/>
+      <c r="CL96" s="414"/>
+      <c r="CM96" s="414"/>
+      <c r="CN96" s="414"/>
+      <c r="CO96" s="414"/>
+      <c r="CP96" s="414"/>
+      <c r="CQ96" s="414"/>
+      <c r="CR96" s="414"/>
+      <c r="CS96" s="417"/>
     </row>
     <row r="97" spans="1:105" ht="10.5" customHeight="1">
       <c r="A97" s="126"/>
@@ -22473,28 +22472,28 @@
       <c r="BT97" s="168"/>
       <c r="BU97" s="168"/>
       <c r="BV97" s="94"/>
-      <c r="BW97" s="421"/>
-      <c r="BX97" s="421"/>
-      <c r="BY97" s="421"/>
-      <c r="BZ97" s="421"/>
-      <c r="CA97" s="421"/>
-      <c r="CB97" s="421"/>
-      <c r="CC97" s="421"/>
-      <c r="CD97" s="421"/>
-      <c r="CE97" s="421"/>
-      <c r="CF97" s="421"/>
-      <c r="CG97" s="421"/>
-      <c r="CH97" s="421"/>
-      <c r="CI97" s="421"/>
-      <c r="CJ97" s="421"/>
-      <c r="CK97" s="421"/>
-      <c r="CL97" s="421"/>
-      <c r="CM97" s="421"/>
-      <c r="CN97" s="421"/>
-      <c r="CO97" s="421"/>
-      <c r="CP97" s="421"/>
-      <c r="CQ97" s="421"/>
-      <c r="CR97" s="421"/>
+      <c r="BW97" s="418"/>
+      <c r="BX97" s="418"/>
+      <c r="BY97" s="418"/>
+      <c r="BZ97" s="418"/>
+      <c r="CA97" s="418"/>
+      <c r="CB97" s="418"/>
+      <c r="CC97" s="418"/>
+      <c r="CD97" s="418"/>
+      <c r="CE97" s="418"/>
+      <c r="CF97" s="418"/>
+      <c r="CG97" s="418"/>
+      <c r="CH97" s="418"/>
+      <c r="CI97" s="418"/>
+      <c r="CJ97" s="418"/>
+      <c r="CK97" s="418"/>
+      <c r="CL97" s="418"/>
+      <c r="CM97" s="418"/>
+      <c r="CN97" s="418"/>
+      <c r="CO97" s="418"/>
+      <c r="CP97" s="418"/>
+      <c r="CQ97" s="418"/>
+      <c r="CR97" s="418"/>
       <c r="CS97" s="178"/>
     </row>
     <row r="98" spans="1:105" ht="10.5" customHeight="1">
@@ -24723,27 +24722,27 @@
         <v>81</v>
       </c>
       <c r="BX119" s="319"/>
-      <c r="BY119" s="418" t="s">
+      <c r="BY119" s="415" t="s">
         <v>83</v>
       </c>
-      <c r="BZ119" s="418"/>
-      <c r="CA119" s="418"/>
-      <c r="CB119" s="418"/>
-      <c r="CC119" s="418"/>
-      <c r="CD119" s="418"/>
-      <c r="CE119" s="418"/>
-      <c r="CF119" s="418"/>
-      <c r="CG119" s="418"/>
-      <c r="CH119" s="418"/>
-      <c r="CI119" s="418"/>
-      <c r="CJ119" s="418"/>
-      <c r="CK119" s="418"/>
-      <c r="CL119" s="418"/>
-      <c r="CM119" s="418"/>
-      <c r="CN119" s="418"/>
-      <c r="CO119" s="418"/>
-      <c r="CP119" s="418"/>
-      <c r="CQ119" s="418"/>
+      <c r="BZ119" s="415"/>
+      <c r="CA119" s="415"/>
+      <c r="CB119" s="415"/>
+      <c r="CC119" s="415"/>
+      <c r="CD119" s="415"/>
+      <c r="CE119" s="415"/>
+      <c r="CF119" s="415"/>
+      <c r="CG119" s="415"/>
+      <c r="CH119" s="415"/>
+      <c r="CI119" s="415"/>
+      <c r="CJ119" s="415"/>
+      <c r="CK119" s="415"/>
+      <c r="CL119" s="415"/>
+      <c r="CM119" s="415"/>
+      <c r="CN119" s="415"/>
+      <c r="CO119" s="415"/>
+      <c r="CP119" s="415"/>
+      <c r="CQ119" s="415"/>
       <c r="CR119" s="80"/>
       <c r="CS119" s="81"/>
       <c r="DI119" s="114"/>
@@ -24824,27 +24823,27 @@
       <c r="BT120" s="58"/>
       <c r="BU120" s="58"/>
       <c r="BV120" s="82"/>
-      <c r="BW120" s="422"/>
-      <c r="BX120" s="422"/>
-      <c r="BY120" s="419"/>
-      <c r="BZ120" s="419"/>
-      <c r="CA120" s="419"/>
-      <c r="CB120" s="419"/>
-      <c r="CC120" s="419"/>
-      <c r="CD120" s="419"/>
-      <c r="CE120" s="419"/>
-      <c r="CF120" s="419"/>
-      <c r="CG120" s="419"/>
-      <c r="CH120" s="419"/>
-      <c r="CI120" s="419"/>
-      <c r="CJ120" s="419"/>
-      <c r="CK120" s="419"/>
-      <c r="CL120" s="419"/>
-      <c r="CM120" s="419"/>
-      <c r="CN120" s="419"/>
-      <c r="CO120" s="419"/>
-      <c r="CP120" s="419"/>
-      <c r="CQ120" s="419"/>
+      <c r="BW120" s="419"/>
+      <c r="BX120" s="419"/>
+      <c r="BY120" s="416"/>
+      <c r="BZ120" s="416"/>
+      <c r="CA120" s="416"/>
+      <c r="CB120" s="416"/>
+      <c r="CC120" s="416"/>
+      <c r="CD120" s="416"/>
+      <c r="CE120" s="416"/>
+      <c r="CF120" s="416"/>
+      <c r="CG120" s="416"/>
+      <c r="CH120" s="416"/>
+      <c r="CI120" s="416"/>
+      <c r="CJ120" s="416"/>
+      <c r="CK120" s="416"/>
+      <c r="CL120" s="416"/>
+      <c r="CM120" s="416"/>
+      <c r="CN120" s="416"/>
+      <c r="CO120" s="416"/>
+      <c r="CP120" s="416"/>
+      <c r="CQ120" s="416"/>
       <c r="CR120" s="83"/>
       <c r="CS120" s="84"/>
     </row>
@@ -24928,31 +24927,31 @@
       <c r="BT121" s="58"/>
       <c r="BU121" s="58"/>
       <c r="BV121" s="82"/>
-      <c r="BW121" s="417" t="s">
+      <c r="BW121" s="414" t="s">
         <v>80</v>
       </c>
-      <c r="BX121" s="417"/>
-      <c r="BY121" s="417"/>
-      <c r="BZ121" s="417"/>
-      <c r="CA121" s="417"/>
-      <c r="CB121" s="417"/>
-      <c r="CC121" s="417"/>
-      <c r="CD121" s="417"/>
-      <c r="CE121" s="417"/>
-      <c r="CF121" s="417"/>
-      <c r="CG121" s="417"/>
-      <c r="CH121" s="417"/>
-      <c r="CI121" s="417"/>
-      <c r="CJ121" s="417"/>
-      <c r="CK121" s="417"/>
-      <c r="CL121" s="417"/>
-      <c r="CM121" s="417"/>
-      <c r="CN121" s="417"/>
-      <c r="CO121" s="417"/>
-      <c r="CP121" s="417"/>
-      <c r="CQ121" s="417"/>
-      <c r="CR121" s="417"/>
-      <c r="CS121" s="420"/>
+      <c r="BX121" s="414"/>
+      <c r="BY121" s="414"/>
+      <c r="BZ121" s="414"/>
+      <c r="CA121" s="414"/>
+      <c r="CB121" s="414"/>
+      <c r="CC121" s="414"/>
+      <c r="CD121" s="414"/>
+      <c r="CE121" s="414"/>
+      <c r="CF121" s="414"/>
+      <c r="CG121" s="414"/>
+      <c r="CH121" s="414"/>
+      <c r="CI121" s="414"/>
+      <c r="CJ121" s="414"/>
+      <c r="CK121" s="414"/>
+      <c r="CL121" s="414"/>
+      <c r="CM121" s="414"/>
+      <c r="CN121" s="414"/>
+      <c r="CO121" s="414"/>
+      <c r="CP121" s="414"/>
+      <c r="CQ121" s="414"/>
+      <c r="CR121" s="414"/>
+      <c r="CS121" s="417"/>
     </row>
     <row r="122" spans="1:151" ht="10.5" customHeight="1">
       <c r="A122" s="126"/>
@@ -25032,28 +25031,28 @@
       <c r="BT122" s="168"/>
       <c r="BU122" s="168"/>
       <c r="BV122" s="94"/>
-      <c r="BW122" s="421"/>
-      <c r="BX122" s="421"/>
-      <c r="BY122" s="421"/>
-      <c r="BZ122" s="421"/>
-      <c r="CA122" s="421"/>
-      <c r="CB122" s="421"/>
-      <c r="CC122" s="421"/>
-      <c r="CD122" s="421"/>
-      <c r="CE122" s="421"/>
-      <c r="CF122" s="421"/>
-      <c r="CG122" s="421"/>
-      <c r="CH122" s="421"/>
-      <c r="CI122" s="421"/>
-      <c r="CJ122" s="421"/>
-      <c r="CK122" s="421"/>
-      <c r="CL122" s="421"/>
-      <c r="CM122" s="421"/>
-      <c r="CN122" s="421"/>
-      <c r="CO122" s="421"/>
-      <c r="CP122" s="421"/>
-      <c r="CQ122" s="421"/>
-      <c r="CR122" s="421"/>
+      <c r="BW122" s="418"/>
+      <c r="BX122" s="418"/>
+      <c r="BY122" s="418"/>
+      <c r="BZ122" s="418"/>
+      <c r="CA122" s="418"/>
+      <c r="CB122" s="418"/>
+      <c r="CC122" s="418"/>
+      <c r="CD122" s="418"/>
+      <c r="CE122" s="418"/>
+      <c r="CF122" s="418"/>
+      <c r="CG122" s="418"/>
+      <c r="CH122" s="418"/>
+      <c r="CI122" s="418"/>
+      <c r="CJ122" s="418"/>
+      <c r="CK122" s="418"/>
+      <c r="CL122" s="418"/>
+      <c r="CM122" s="418"/>
+      <c r="CN122" s="418"/>
+      <c r="CO122" s="418"/>
+      <c r="CP122" s="418"/>
+      <c r="CQ122" s="418"/>
+      <c r="CR122" s="418"/>
       <c r="CS122" s="178"/>
     </row>
     <row r="123" spans="1:151" ht="10.5" customHeight="1">

</xml_diff>